<commit_message>
add supervisor phone in import sheet
</commit_message>
<xml_diff>
--- a/public/imports/Clients_with_relatives.xlsx
+++ b/public/imports/Clients_with_relatives.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Alraqiah\public\imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\promo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -55,6 +55,27 @@
   </si>
   <si>
     <t>launch_date</t>
+  </si>
+  <si>
+    <t>supervisor_phone</t>
+  </si>
+  <si>
+    <t>mohamed hamada</t>
+  </si>
+  <si>
+    <t>egypt</t>
+  </si>
+  <si>
+    <t>nasser</t>
+  </si>
+  <si>
+    <t>022222</t>
+  </si>
+  <si>
+    <t>01101865213</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -64,13 +85,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,14 +120,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     </dxf>
@@ -118,19 +153,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J1048571" totalsRowShown="0">
-  <autoFilter ref="A1:J1048571"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K1048571" totalsRowShown="0">
+  <autoFilter ref="A1:K1048571"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="name"/>
-    <tableColumn id="2" name="phone"/>
+    <tableColumn id="2" name="phone" dataDxfId="0"/>
     <tableColumn id="3" name="reservation_number"/>
     <tableColumn id="4" name="package"/>
-    <tableColumn id="5" name="launch_date" dataDxfId="0"/>
+    <tableColumn id="5" name="launch_date" dataDxfId="2"/>
     <tableColumn id="6" name="seat_number"/>
     <tableColumn id="7" name="gender"/>
     <tableColumn id="8" name="identity_number"/>
     <tableColumn id="9" name="country"/>
     <tableColumn id="10" name="incoming_city"/>
+    <tableColumn id="11" name="supervisor_phone" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -415,16 +451,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="2" max="2" width="25" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
@@ -433,14 +469,14 @@
     <col min="8" max="8" width="26.5703125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -467,8 +503,51 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>2512</v>
+      </c>
+      <c r="D2">
+        <v>4511</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45409</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>8752565</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+      <formula1>"male,female"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -481,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +600,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>"male,female"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
add arrival_location_url in import clients
</commit_message>
<xml_diff>
--- a/public/imports/Clients_with_relatives.xlsx
+++ b/public/imports/Clients_with_relatives.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>chronic_disease_discription</t>
+  </si>
+  <si>
+    <t>arrival_location_url</t>
+  </si>
+  <si>
+    <t>chronic_disease_description</t>
   </si>
 </sst>
 </file>
@@ -134,9 +140,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M1047180" totalsRowShown="0">
-  <autoFilter ref="A1:M1047180"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:N1047179" totalsRowShown="0">
+  <autoFilter ref="A1:N1047179"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="name"/>
     <tableColumn id="2" name="phone" dataDxfId="2"/>
     <tableColumn id="3" name="reservation_number"/>
@@ -149,7 +155,8 @@
     <tableColumn id="10" name="incoming_city"/>
     <tableColumn id="11" name="supervisor_phone" dataDxfId="0"/>
     <tableColumn id="12" name="chronic_disease"/>
-    <tableColumn id="13" name="chronic_disease_discription"/>
+    <tableColumn id="13" name="chronic_disease_description"/>
+    <tableColumn id="14" name="arrival_location_url"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,9 +464,10 @@
     <col min="11" max="11" width="21.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
     <col min="13" max="13" width="32.28515625" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +505,10 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -521,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>